<commit_message>
added results to excel
</commit_message>
<xml_diff>
--- a/performances.xlsx
+++ b/performances.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malteebner/Library/Mobile Documents/com~apple~CloudDocs/Master ETIT/10. Semester/Forschungsarbeit/Code Forschungsarbeit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A3FD8A-2FE3-B844-8E7D-FB85F395745D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8E5BF7-8594-2946-99E3-192BE8ECD8E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16680" xr2:uid="{0C047C73-2AED-574F-B05A-862A7DD3D487}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="16680" xr2:uid="{0C047C73-2AED-574F-B05A-862A7DD3D487}"/>
   </bookViews>
   <sheets>
     <sheet name="refinery_results" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="49">
   <si>
     <t>BatchSize</t>
   </si>
@@ -150,9 +150,6 @@
   </si>
   <si>
     <t>human - std</t>
-  </si>
-  <si>
-    <t>genetic</t>
   </si>
   <si>
     <t>calculation duration</t>
@@ -549,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{358AB6D0-DA15-D244-B588-E9E7D3C401A4}">
-  <dimension ref="A2:I50"/>
+  <dimension ref="A2:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -585,10 +582,10 @@
         <v>23</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="16" x14ac:dyDescent="0.2">
@@ -808,7 +805,7 @@
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C15" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D15" s="4">
         <f>E15*F15</f>
@@ -864,7 +861,7 @@
     </row>
     <row r="19" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>8</v>
@@ -889,7 +886,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C20" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D20" s="2">
         <f t="shared" ref="D20:D50" si="1">IF(E20*F20&gt;0,E20*F20,"")</f>
@@ -910,7 +907,7 @@
     </row>
     <row r="21" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="C21" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D21" s="2">
         <f t="shared" si="1"/>
@@ -932,17 +929,17 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C22" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D22" s="2">
         <f t="shared" si="1"/>
-        <v>903952095</v>
+        <v>813981250</v>
       </c>
       <c r="E22" s="2">
-        <v>345</v>
+        <v>326</v>
       </c>
       <c r="F22" s="2">
-        <v>2620151</v>
+        <v>2496875</v>
       </c>
       <c r="H22" s="2">
         <v>4111</v>
@@ -1003,10 +1000,10 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D26" s="2">
         <f t="shared" si="1"/>
@@ -1027,22 +1024,28 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C27" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D27" s="2">
         <f t="shared" si="1"/>
-        <v>3058520850</v>
+        <v>809758246</v>
       </c>
       <c r="E27" s="2">
-        <v>770</v>
+        <v>326</v>
       </c>
       <c r="F27" s="2">
-        <v>3972105</v>
+        <v>2483921</v>
+      </c>
+      <c r="H27" s="2">
+        <v>985</v>
+      </c>
+      <c r="I27" s="2">
+        <v>3000</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C28" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D28" s="2">
         <f t="shared" si="1"/>
@@ -1111,10 +1114,10 @@
     </row>
     <row r="32" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="D32" s="2">
         <f t="shared" si="1"/>
@@ -1136,7 +1139,7 @@
     </row>
     <row r="33" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="C33" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D33" s="2">
         <f t="shared" si="1"/>
@@ -1158,7 +1161,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C34" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D34" s="2">
         <f t="shared" si="1"/>
@@ -1223,41 +1226,82 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D38" s="2" t="str">
+        <v>46</v>
+      </c>
+      <c r="D38" s="2">
         <f t="shared" si="1"/>
-        <v/>
+        <v>1064059425</v>
+      </c>
+      <c r="E38" s="2">
+        <v>275</v>
+      </c>
+      <c r="F38" s="2">
+        <v>3869307</v>
+      </c>
+      <c r="H38" s="2">
+        <v>5011</v>
+      </c>
+      <c r="I38" s="2">
+        <v>10000</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C39" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D39" s="2" t="str">
+        <v>40</v>
+      </c>
+      <c r="D39" s="2">
         <f t="shared" si="1"/>
-        <v/>
+        <v>809521622</v>
+      </c>
+      <c r="E39" s="2">
+        <v>254</v>
+      </c>
+      <c r="F39" s="2">
+        <v>3187093</v>
+      </c>
+      <c r="H39" s="2">
+        <v>996</v>
+      </c>
+      <c r="I39" s="2">
+        <v>3000</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C40" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D40" s="2" t="str">
+        <v>41</v>
+      </c>
+      <c r="D40" s="2">
         <f t="shared" si="1"/>
-        <v/>
+        <v>909745990</v>
+      </c>
+      <c r="E40" s="2">
+        <v>289</v>
+      </c>
+      <c r="F40" s="2">
+        <v>3147910</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C41" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D41" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="D41" s="2">
+        <v>783915168</v>
+      </c>
+      <c r="E41" s="2">
+        <v>251</v>
+      </c>
+      <c r="F41" s="2">
+        <v>3123168</v>
+      </c>
+      <c r="H41" s="2">
+        <v>582</v>
+      </c>
+      <c r="I41" s="2">
+        <v>231000</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
@@ -1287,51 +1331,9 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D44" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D45" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D46" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D47" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D48" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D49" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D50" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
   </sheetData>
   <conditionalFormatting sqref="G32:G33 G23:G24 G3:G14 G16:G19">
-    <cfRule type="dataBar" priority="40">
+    <cfRule type="dataBar" priority="49">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1345,7 +1347,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G21">
-    <cfRule type="dataBar" priority="14">
+    <cfRule type="dataBar" priority="23">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1358,8 +1360,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D21 D45">
-    <cfRule type="colorScale" priority="15">
+  <conditionalFormatting sqref="D21">
+    <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1371,7 +1373,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="colorScale" priority="16">
+    <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1383,7 +1385,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F21">
-    <cfRule type="colorScale" priority="17">
+    <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1395,7 +1397,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27">
-    <cfRule type="colorScale" priority="8">
+    <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1407,7 +1409,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E27">
-    <cfRule type="colorScale" priority="9">
+    <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1419,7 +1421,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F27">
-    <cfRule type="colorScale" priority="10">
+    <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1430,8 +1432,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D28:D29 D26 D50">
-    <cfRule type="colorScale" priority="11">
+  <conditionalFormatting sqref="D28:D29 D26">
+    <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1443,7 +1445,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28:E29 E26">
-    <cfRule type="colorScale" priority="12">
+    <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1455,7 +1457,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28:F29 F26">
-    <cfRule type="colorScale" priority="13">
+    <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1466,8 +1468,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D19:D50">
-    <cfRule type="colorScale" priority="99">
+  <conditionalFormatting sqref="D19:D43">
+    <cfRule type="colorScale" priority="108">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1479,7 +1481,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E32:E36 E42 E22:E24 E30 E19:E20">
-    <cfRule type="colorScale" priority="104">
+    <cfRule type="colorScale" priority="113">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1491,7 +1493,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F32:F36 F42 F22:F24 F30 F19:F20">
-    <cfRule type="colorScale" priority="109">
+    <cfRule type="colorScale" priority="118">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1503,7 +1505,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D38:D41">
-    <cfRule type="colorScale" priority="5">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1515,7 +1517,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E38:E41">
-    <cfRule type="colorScale" priority="6">
+    <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1527,7 +1529,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F38:F41">
-    <cfRule type="colorScale" priority="7">
+    <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1538,8 +1540,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D19:D50">
-    <cfRule type="colorScale" priority="3">
+  <conditionalFormatting sqref="D19:D43">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1551,7 +1553,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19:E42">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1563,6 +1565,114 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F19:F42">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D44:D54">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E44:E48 E54">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F44:F48 F54">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D50:D53">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E50:E53">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F50:F53">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D44:D54">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E44:E54">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F44:F54">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -1612,16 +1722,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE22436E-1B01-4E4E-82EB-F6524F9BD974}">
-  <dimension ref="C4:O24"/>
+  <dimension ref="C4:O32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1655,10 +1765,10 @@
         <v>35</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="3:15" x14ac:dyDescent="0.2">
@@ -1756,112 +1866,181 @@
       <c r="M8" s="1"/>
     </row>
     <row r="9" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="E9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="1">
+      <c r="C9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="1">
+        <v>62.59</v>
+      </c>
+      <c r="G11" s="1">
+        <v>53.33</v>
+      </c>
+      <c r="H11" s="1">
+        <v>53</v>
+      </c>
+      <c r="I11" s="1">
+        <v>67.22</v>
+      </c>
+      <c r="J11" s="1">
+        <v>72</v>
+      </c>
+      <c r="K11" s="1">
+        <v>67</v>
+      </c>
+      <c r="L11" s="1">
+        <v>63</v>
+      </c>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1">
+        <v>3543</v>
+      </c>
+      <c r="O11" s="1">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="12" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="1">
+        <v>64.290000000000006</v>
+      </c>
+      <c r="G12" s="1">
+        <v>53.33</v>
+      </c>
+      <c r="H12" s="1">
+        <v>53.2</v>
+      </c>
+      <c r="I12" s="1">
+        <v>72.22</v>
+      </c>
+      <c r="J12" s="1">
+        <v>76</v>
+      </c>
+      <c r="K12" s="1">
+        <v>66</v>
+      </c>
+      <c r="L12" s="1">
+        <v>65</v>
+      </c>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1">
+        <v>1354</v>
+      </c>
+      <c r="O12" s="1">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="13" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="1">
         <v>65.05</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G13" s="1">
         <v>53.333329999999997</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H13" s="1">
         <v>52.2</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I13" s="1">
         <v>72.777777700000001</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J13" s="1">
         <v>78</v>
       </c>
-      <c r="K9" s="1">
+      <c r="K13" s="1">
         <v>69</v>
       </c>
-      <c r="L9" s="1">
+      <c r="L13" s="1">
         <v>65</v>
       </c>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1">
+      <c r="M13" s="1"/>
+      <c r="N13" s="1">
         <v>1654</v>
       </c>
-      <c r="O9" s="1">
+      <c r="O13" s="1">
         <v>1600</v>
       </c>
     </row>
-    <row r="10" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="E10" t="s">
+    <row r="14" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F14" s="1">
         <v>65.040000000000006</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G14" s="1">
         <v>53.33</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H14" s="1">
         <v>52.6</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I14" s="1">
         <v>73.33</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J14" s="1">
         <v>77</v>
       </c>
-      <c r="K10" s="1">
+      <c r="K14" s="1">
         <v>69</v>
       </c>
-      <c r="L10" s="1">
+      <c r="L14" s="1">
         <v>65</v>
       </c>
-      <c r="M10" s="1"/>
-      <c r="N10">
+      <c r="M14" s="1"/>
+      <c r="N14">
         <v>2385</v>
       </c>
-      <c r="O10">
+      <c r="O14">
         <v>8192</v>
       </c>
     </row>
-    <row r="11" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-    </row>
-    <row r="12" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-    </row>
-    <row r="13" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-    </row>
-    <row r="14" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-    </row>
     <row r="15" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -1872,6 +2051,13 @@
       <c r="M15" s="1"/>
     </row>
     <row r="16" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -1881,7 +2067,12 @@
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="6:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -1891,7 +2082,12 @@
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="6:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -1901,7 +2097,12 @@
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
     </row>
-    <row r="19" spans="6:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -1911,7 +2112,12 @@
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
     </row>
-    <row r="20" spans="6:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -1921,7 +2127,10 @@
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
     </row>
-    <row r="21" spans="6:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -1931,35 +2140,84 @@
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
     </row>
-    <row r="22" spans="6:13" x14ac:dyDescent="0.2">
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-    </row>
-    <row r="23" spans="6:13" x14ac:dyDescent="0.2">
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-    </row>
-    <row r="24" spans="6:13" x14ac:dyDescent="0.2">
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
+    <row r="22" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C22" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C28" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>